<commit_message>
LIBRA : end ch2
</commit_message>
<xml_diff>
--- a/DataEngineering/DataProcessing/LIBRA/DataNote.xlsx
+++ b/DataEngineering/DataProcessing/LIBRA/DataNote.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jung_yujin/workspace/TIL/DataEngineering/DataProcessing/LIBRA/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E8964C9-3791-3342-97ED-2B0B33F118F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF93A3EF-EA7B-0741-8A12-BF460C6CA544}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14400" yWindow="500" windowWidth="14400" windowHeight="15720" xr2:uid="{F15BF391-CD1F-1D46-9B78-03CD17453F69}"/>
+    <workbookView xWindow="4480" yWindow="1060" windowWidth="14400" windowHeight="15720" xr2:uid="{F15BF391-CD1F-1D46-9B78-03CD17453F69}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -159,14 +159,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t xml:space="preserve">- 의료, 음/식료품, </t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>- 여행/교통, 미용, 의류/잡화, 요식/유흥, 스포츠/문화/레저</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>total 500, unique 498 &gt;&gt; drop</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -175,16 +167,7 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>target : 카드이용금액계 ?</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>결측치 없음, 아래 두 데이터에 각각 병합</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>New feature : COVID 발생 여부 (Boolean)
-int형이 아닌 datetime object로</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -207,7 +190,27 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>New feature : 카드이용건수 중 10대의 비율</t>
+    <t>New feature : 카드이용건수 중 10대의 비율
+New feature : 가장 많은 연령층(=40대)의 카드이용건수</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>target : 소액결제건수</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>New feature
+: 국내 COVID 확진자 발생 여부 (Boolean)
+int형이 아닌 datetime object로</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>New feature
+: 서울시 추가 확진자 수 데이터 (월별)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>- 요식/유흥, 유통, 의료 (데이터 수가 10개 이상인 업종)</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -339,7 +342,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -389,6 +392,9 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -399,9 +405,9 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FFB26CFF"/>
       <color rgb="FFC3BFFE"/>
       <color rgb="FFC3B3FE"/>
-      <color rgb="FFB26CFF"/>
     </mruColors>
   </colors>
   <extLst>
@@ -714,8 +720,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C4382004-1911-3246-85AC-5288D671F973}">
   <dimension ref="A1:G29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18"/>
@@ -733,7 +739,7 @@
         <v>29</v>
       </c>
       <c r="C1" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
     </row>
     <row r="2" spans="1:7">
@@ -797,7 +803,7 @@
       <c r="F8" s="3"/>
       <c r="G8" s="3"/>
     </row>
-    <row r="9" spans="1:7" ht="40" customHeight="1">
+    <row r="9" spans="1:7" ht="53" customHeight="1">
       <c r="A9" s="8" t="s">
         <v>4</v>
       </c>
@@ -816,7 +822,7 @@
         <v>18</v>
       </c>
       <c r="C10" s="12" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="11" spans="1:7">
@@ -827,15 +833,15 @@
         <v>19</v>
       </c>
     </row>
-    <row r="12" spans="1:7">
+    <row r="12" spans="1:7" ht="57">
       <c r="A12" s="7" t="s">
         <v>7</v>
       </c>
       <c r="B12" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="C12" s="7" t="s">
-        <v>38</v>
+      <c r="C12" s="17" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="32" customHeight="1">
@@ -846,10 +852,10 @@
         <v>18</v>
       </c>
       <c r="C13" s="16" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="34" customHeight="1">
       <c r="A14" s="3" t="s">
         <v>9</v>
       </c>
@@ -907,7 +913,7 @@
         <v>18</v>
       </c>
       <c r="C20" s="12" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="21" spans="1:3">
@@ -930,6 +936,9 @@
       <c r="A24" s="7" t="s">
         <v>20</v>
       </c>
+      <c r="C24" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="25" spans="1:3">
       <c r="A25" s="2" t="s">
@@ -941,24 +950,22 @@
         <v>22</v>
       </c>
     </row>
-    <row r="27" spans="1:3">
+    <row r="27" spans="1:3" ht="38">
       <c r="A27" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="C27" t="s">
-        <v>34</v>
+      <c r="C27" s="15" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="28" spans="1:3">
       <c r="A28" s="11" t="s">
-        <v>30</v>
+        <v>38</v>
       </c>
       <c r="C28" s="10"/>
     </row>
     <row r="29" spans="1:3">
-      <c r="A29" s="11" t="s">
-        <v>31</v>
-      </c>
+      <c r="A29" s="11"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>